<commit_message>
messing around with input
</commit_message>
<xml_diff>
--- a/datasets/things.xlsx
+++ b/datasets/things.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,34 @@
       <c r="F2" t="inlineStr">
         <is>
           <t>work experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>b979ba9a-87ca-4b10-9b53-48dd201ed68a</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01/02/2023</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Xmas 2022</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Xmas 2022</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Xmas vacation 2022</t>
         </is>
       </c>
     </row>
@@ -691,20 +719,14 @@
           <t>description</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>TRUE</t>
-        </is>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>